<commit_message>
trying to publish the app
</commit_message>
<xml_diff>
--- a/CICES/CICES-Questionnaire.xlsx
+++ b/CICES/CICES-Questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/4-Projects/everest-bio-tool/CICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A589D2C1-83AB-984D-9A9A-A9A52F47D84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1A24D1-26F1-5D4D-8E16-92B9B6F6DE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="874">
   <si>
     <t>Division</t>
   </si>
@@ -2783,7 +2783,97 @@
     <t>Is the Genetic material from plants, algae or fungi (including seed, spore or gamete production) affected by the use of your technology int the territory ?</t>
   </si>
   <si>
-    <t>Seeds, Spores</t>
+    <t>Plantes</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Other types?</t>
+  </si>
+  <si>
+    <t>ProvidingOthers</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Is the Transformation of biochemical or physical inputs to ecosystems an issue?</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Your technology transform  biochemical or physical inputs to the ecosystems ?</t>
+  </si>
+  <si>
+    <t>Animals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toxic substances of anthropogenic origin </t>
+  </si>
+  <si>
+    <t>Nuisances of anthropogenic origin</t>
+  </si>
+  <si>
+    <t>Is the regulation of physical, chemical, biological conditions an issue for the territory?</t>
+  </si>
+  <si>
+    <t>have your technology an impact on the regulation of physical, chemical, biological conditions for the territory?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the cultural dimension an important element of the territory? </t>
+  </si>
+  <si>
+    <t>Do you think that your technology can affect/influence the cultural dimensions of the Ecosystem?</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Intellectual interactions with Natural environment</t>
+  </si>
+  <si>
+    <t>Spiritual, symbolic interactions with Natural environment</t>
+  </si>
+  <si>
+    <t>Surface water</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Is Water (for nutrition, materials or energy) an issue for the territory?</t>
+  </si>
+  <si>
+    <t>Is the Water (as a Nutrition, Material or Energy asset) impacted  beacause of your technology?</t>
+  </si>
+  <si>
+    <t>Ground Water</t>
+  </si>
+  <si>
+    <t>Other aqueous ecosystems</t>
+  </si>
+  <si>
+    <t>Regulation of baseline flows</t>
+  </si>
+  <si>
+    <t>Pest and Disease</t>
+  </si>
+  <si>
+    <t>Water conditions</t>
+  </si>
+  <si>
+    <t>Other regulation and maintenance services</t>
+  </si>
+  <si>
+    <t>Physical and experiential interactions with Nature</t>
+  </si>
+  <si>
+    <t>Other Biotic charasteristics with non use value</t>
+  </si>
+  <si>
+    <t>Other cultural significance</t>
   </si>
 </sst>
 </file>
@@ -2793,7 +2883,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2983,6 +3073,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -3789,7 +3885,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="416">
+  <cellXfs count="417">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5022,6 +5118,7 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5642,8 +5739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="D63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -7122,6 +7219,9 @@
       </c>
     </row>
     <row r="27" spans="2:26" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="265" t="s">
+        <v>851</v>
+      </c>
       <c r="F27" s="55" t="s">
         <v>28</v>
       </c>
@@ -7303,6 +7403,18 @@
       </c>
     </row>
     <row r="30" spans="2:26" ht="146.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="265" t="s">
+        <v>845</v>
+      </c>
+      <c r="C30" s="265" t="s">
+        <v>845</v>
+      </c>
+      <c r="D30" s="265" t="s">
+        <v>844</v>
+      </c>
+      <c r="E30" s="265" t="s">
+        <v>846</v>
+      </c>
       <c r="F30" s="250" t="s">
         <v>28</v>
       </c>
@@ -7354,6 +7466,18 @@
       </c>
     </row>
     <row r="31" spans="2:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="265" t="s">
+        <v>848</v>
+      </c>
+      <c r="C31" s="265" t="s">
+        <v>850</v>
+      </c>
+      <c r="D31" s="265" t="s">
+        <v>847</v>
+      </c>
+      <c r="E31" s="265" t="s">
+        <v>852</v>
+      </c>
       <c r="F31" s="7" t="s">
         <v>28</v>
       </c>
@@ -7477,7 +7601,10 @@
         <v>749</v>
       </c>
     </row>
-    <row r="33" spans="6:26" ht="253.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:26" ht="253.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="265" t="s">
+        <v>853</v>
+      </c>
       <c r="F33" s="16" t="s">
         <v>28</v>
       </c>
@@ -7538,7 +7665,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="34" spans="6:26" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:26" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="16" t="s">
         <v>28</v>
       </c>
@@ -7601,7 +7728,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="35" spans="6:26" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:26" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F35" s="245" t="s">
         <v>28</v>
       </c>
@@ -7662,7 +7789,19 @@
         <v>733</v>
       </c>
     </row>
-    <row r="36" spans="6:26" ht="186.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:26" ht="186.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="265" t="s">
+        <v>854</v>
+      </c>
+      <c r="C36" s="265" t="s">
+        <v>855</v>
+      </c>
+      <c r="D36" s="265" t="s">
+        <v>849</v>
+      </c>
+      <c r="E36" s="265" t="s">
+        <v>867</v>
+      </c>
       <c r="F36" s="32" t="s">
         <v>28</v>
       </c>
@@ -7725,7 +7864,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="37" spans="6:26" ht="100" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:26" ht="100" x14ac:dyDescent="0.2">
       <c r="F37" s="16" t="s">
         <v>28</v>
       </c>
@@ -7786,7 +7925,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="38" spans="6:26" ht="321" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:26" ht="321" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F38" s="16" t="s">
         <v>28</v>
       </c>
@@ -7849,7 +7988,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="39" spans="6:26" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:26" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="55" t="s">
         <v>28</v>
       </c>
@@ -7912,7 +8051,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="40" spans="6:26" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:26" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F40" s="245" t="s">
         <v>28</v>
       </c>
@@ -7975,7 +8114,10 @@
         <v>752</v>
       </c>
     </row>
-    <row r="41" spans="6:26" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:26" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="265" t="s">
+        <v>176</v>
+      </c>
       <c r="F41" s="250" t="s">
         <v>28</v>
       </c>
@@ -8038,7 +8180,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="42" spans="6:26" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:26" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" s="32" t="s">
         <v>28</v>
       </c>
@@ -8101,7 +8243,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="43" spans="6:26" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:26" ht="161" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F43" s="179" t="s">
         <v>28</v>
       </c>
@@ -8164,7 +8306,10 @@
         <v>753</v>
       </c>
     </row>
-    <row r="44" spans="6:26" ht="220" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:26" ht="220" x14ac:dyDescent="0.15">
+      <c r="E44" s="416" t="s">
+        <v>868</v>
+      </c>
       <c r="F44" s="7" t="s">
         <v>28</v>
       </c>
@@ -8227,7 +8372,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="45" spans="6:26" ht="141" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:26" ht="141" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F45" s="157" t="s">
         <v>28</v>
       </c>
@@ -8290,7 +8435,10 @@
         <v>753</v>
       </c>
     </row>
-    <row r="46" spans="6:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:26" ht="80" x14ac:dyDescent="0.2">
+      <c r="E46" s="265" t="s">
+        <v>220</v>
+      </c>
       <c r="F46" s="32" t="s">
         <v>28</v>
       </c>
@@ -8351,7 +8499,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="47" spans="6:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F47" s="245" t="s">
         <v>28</v>
       </c>
@@ -8412,7 +8560,10 @@
         <v>754</v>
       </c>
     </row>
-    <row r="48" spans="6:26" ht="212.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:26" ht="212.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="265" t="s">
+        <v>869</v>
+      </c>
       <c r="F48" s="244" t="s">
         <v>28</v>
       </c>
@@ -8475,7 +8626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="6:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F49" s="245" t="s">
         <v>28</v>
       </c>
@@ -8538,7 +8689,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="6:26" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:26" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="265" t="s">
+        <v>255</v>
+      </c>
       <c r="F50" s="244" t="s">
         <v>28</v>
       </c>
@@ -8601,7 +8755,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="51" spans="6:26" ht="238.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:26" ht="238.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F51" s="245" t="s">
         <v>28</v>
       </c>
@@ -8664,7 +8818,10 @@
         <v>755</v>
       </c>
     </row>
-    <row r="52" spans="6:26" ht="121" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:26" ht="121" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="265" t="s">
+        <v>870</v>
+      </c>
       <c r="F52" s="250" t="s">
         <v>28</v>
       </c>
@@ -8715,7 +8872,19 @@
         <v>731</v>
       </c>
     </row>
-    <row r="53" spans="6:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="265" t="s">
+        <v>856</v>
+      </c>
+      <c r="C53" s="265" t="s">
+        <v>857</v>
+      </c>
+      <c r="D53" s="265" t="s">
+        <v>858</v>
+      </c>
+      <c r="E53" s="265" t="s">
+        <v>871</v>
+      </c>
       <c r="F53" s="7" t="s">
         <v>28</v>
       </c>
@@ -8776,7 +8945,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="54" spans="6:26" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:26" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F54" s="245" t="s">
         <v>28</v>
       </c>
@@ -8839,7 +9008,10 @@
         <v>743</v>
       </c>
     </row>
-    <row r="55" spans="6:26" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:26" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E55" s="265" t="s">
+        <v>859</v>
+      </c>
       <c r="F55" s="244" t="s">
         <v>28</v>
       </c>
@@ -8900,7 +9072,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="56" spans="6:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:26" ht="80" x14ac:dyDescent="0.2">
       <c r="F56" s="16" t="s">
         <v>28</v>
       </c>
@@ -8961,7 +9133,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="57" spans="6:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:26" ht="80" x14ac:dyDescent="0.2">
       <c r="F57" s="16" t="s">
         <v>28</v>
       </c>
@@ -9022,7 +9194,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="58" spans="6:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F58" s="157" t="s">
         <v>28</v>
       </c>
@@ -9083,7 +9255,10 @@
         <v>756</v>
       </c>
     </row>
-    <row r="59" spans="6:26" ht="100" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:26" ht="100" x14ac:dyDescent="0.2">
+      <c r="E59" s="265" t="s">
+        <v>860</v>
+      </c>
       <c r="F59" s="7" t="s">
         <v>28</v>
       </c>
@@ -9144,7 +9319,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="60" spans="6:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:26" ht="80" x14ac:dyDescent="0.2">
       <c r="F60" s="16" t="s">
         <v>28</v>
       </c>
@@ -9205,7 +9380,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="61" spans="6:26" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:26" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F61" s="32" t="s">
         <v>28</v>
       </c>
@@ -9266,7 +9441,10 @@
         <v>756</v>
       </c>
     </row>
-    <row r="62" spans="6:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E62" s="265" t="s">
+        <v>872</v>
+      </c>
       <c r="F62" s="16" t="s">
         <v>28</v>
       </c>
@@ -9327,7 +9505,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="63" spans="6:26" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:26" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F63" s="220" t="s">
         <v>28</v>
       </c>
@@ -9388,7 +9566,10 @@
         <v>731</v>
       </c>
     </row>
-    <row r="64" spans="6:26" ht="101" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:26" ht="101" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="265" t="s">
+        <v>873</v>
+      </c>
       <c r="F64" s="32" t="s">
         <v>28</v>
       </c>
@@ -9439,7 +9620,19 @@
         <v>731</v>
       </c>
     </row>
-    <row r="65" spans="6:26" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:26" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="265" t="s">
+        <v>863</v>
+      </c>
+      <c r="C65" s="265" t="s">
+        <v>864</v>
+      </c>
+      <c r="D65" s="265" t="s">
+        <v>862</v>
+      </c>
+      <c r="E65" s="265" t="s">
+        <v>861</v>
+      </c>
       <c r="F65" s="71" t="s">
         <v>635</v>
       </c>
@@ -9502,7 +9695,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="66" spans="6:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:26" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F66" s="71" t="s">
         <v>635</v>
       </c>
@@ -9565,7 +9758,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="67" spans="6:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F67" s="71" t="s">
         <v>635</v>
       </c>
@@ -9626,7 +9819,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="6:26" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:26" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F68" s="114" t="s">
         <v>635</v>
       </c>
@@ -9687,7 +9880,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="69" spans="6:26" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:26" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E69" s="265" t="s">
+        <v>865</v>
+      </c>
       <c r="F69" s="71" t="s">
         <v>635</v>
       </c>
@@ -9750,7 +9946,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="70" spans="6:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F70" s="71" t="s">
         <v>635</v>
       </c>
@@ -9813,7 +10009,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="71" spans="6:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F71" s="71" t="s">
         <v>635</v>
       </c>
@@ -9874,7 +10070,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="72" spans="6:26" ht="120" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:26" ht="120" x14ac:dyDescent="0.2">
+      <c r="E72" s="265" t="s">
+        <v>866</v>
+      </c>
       <c r="F72" s="158" t="s">
         <v>635</v>
       </c>
@@ -9925,7 +10124,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="73" spans="6:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:26" ht="80" x14ac:dyDescent="0.2">
       <c r="F73" s="158" t="s">
         <v>379</v>
       </c>
@@ -9986,7 +10185,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="74" spans="6:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:26" ht="80" x14ac:dyDescent="0.2">
       <c r="F74" s="158" t="s">
         <v>379</v>
       </c>
@@ -10047,7 +10246,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="75" spans="6:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F75" s="158" t="s">
         <v>379</v>
       </c>
@@ -10108,7 +10307,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="76" spans="6:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:26" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F76" s="158" t="s">
         <v>379</v>
       </c>
@@ -10169,7 +10368,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="77" spans="6:26" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:26" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F77" s="71" t="s">
         <v>379</v>
       </c>
@@ -10230,7 +10429,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="78" spans="6:26" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:26" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F78" s="71" t="s">
         <v>379</v>
       </c>
@@ -10291,7 +10490,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="79" spans="6:26" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:26" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F79" s="71" t="s">
         <v>379</v>
       </c>
@@ -10352,7 +10551,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="80" spans="6:26" ht="60" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:26" ht="60" x14ac:dyDescent="0.2">
       <c r="F80" s="71" t="s">
         <v>379</v>
       </c>

</xml_diff>